<commit_message>
Implemented fully working flow
</commit_message>
<xml_diff>
--- a/FII_LIST.xlsx
+++ b/FII_LIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://voeazul-my.sharepoint.com/personal/gabriel_bsantos_voeazul_com_br/Documents/Área de Trabalho/Gabriel/ScriptsPy/GitHub/REAL-STATE-FUND-BR-VALOVERDIV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_F463E3DFAFF153DFD89AFCCC9413B6B05E6EE283" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2069C4A4-555E-45B2-AF23-D8102DCAA7DA}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_F463E3DFAFF153DFD89AFCCC9413B6B05E6EE283" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31F78C6F-0809-4D0B-A089-E8C5C340785D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>COD</t>
   </si>
@@ -58,6 +58,63 @@
   </si>
   <si>
     <t>ANCR11</t>
+  </si>
+  <si>
+    <t>AQLL11</t>
+  </si>
+  <si>
+    <t>ARCT11</t>
+  </si>
+  <si>
+    <t>ATCR11</t>
+  </si>
+  <si>
+    <t>ATSA11</t>
+  </si>
+  <si>
+    <t>AURA11</t>
+  </si>
+  <si>
+    <t>BBFI11</t>
+  </si>
+  <si>
+    <t>BBIM11</t>
+  </si>
+  <si>
+    <t>BBPO11</t>
+  </si>
+  <si>
+    <t>BCFF11</t>
+  </si>
+  <si>
+    <t>BCRI11</t>
+  </si>
+  <si>
+    <t>BFIN11</t>
+  </si>
+  <si>
+    <t>BFRM11</t>
+  </si>
+  <si>
+    <t>BMLC11</t>
+  </si>
+  <si>
+    <t>BPCA11</t>
+  </si>
+  <si>
+    <t>BPFF11</t>
+  </si>
+  <si>
+    <t>BPML11</t>
+  </si>
+  <si>
+    <t>BRCR11</t>
+  </si>
+  <si>
+    <t>BRFI11</t>
+  </si>
+  <si>
+    <t>CBOP11</t>
   </si>
 </sst>
 </file>
@@ -118,10 +175,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A11:XFD28"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -485,6 +538,106 @@
         <v>10</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Finished the working product
</commit_message>
<xml_diff>
--- a/FII_LIST.xlsx
+++ b/FII_LIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://voeazul-my.sharepoint.com/personal/gabriel_bsantos_voeazul_com_br/Documents/Área de Trabalho/Gabriel/ScriptsPy/GitHub/REAL-STATE-FUND-BR-VALOVERDIV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_F463E3DFAFF153DFD89AFCCC9413B6B05E6EE283" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31F78C6F-0809-4D0B-A089-E8C5C340785D}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_F463E3DFAFF153DFD89AFCCC9413B6B05E6EE283" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41CA0D9D-6260-4AC5-AA06-F97316304242}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="94">
   <si>
     <t>COD</t>
   </si>
@@ -36,51 +36,21 @@
     <t>ABCP11</t>
   </si>
   <si>
-    <t>ABRD11</t>
-  </si>
-  <si>
     <t>AEFI11</t>
   </si>
   <si>
-    <t>AFOF11</t>
-  </si>
-  <si>
-    <t>AGCX11</t>
-  </si>
-  <si>
     <t>ALMI11</t>
   </si>
   <si>
-    <t>ALMI12</t>
-  </si>
-  <si>
     <t>ALZR11</t>
   </si>
   <si>
-    <t>ANCR11</t>
-  </si>
-  <si>
     <t>AQLL11</t>
   </si>
   <si>
-    <t>ARCT11</t>
-  </si>
-  <si>
-    <t>ATCR11</t>
-  </si>
-  <si>
     <t>ATSA11</t>
   </si>
   <si>
-    <t>AURA11</t>
-  </si>
-  <si>
-    <t>BBFI11</t>
-  </si>
-  <si>
-    <t>BBIM11</t>
-  </si>
-  <si>
     <t>BBPO11</t>
   </si>
   <si>
@@ -90,18 +60,9 @@
     <t>BCRI11</t>
   </si>
   <si>
-    <t>BFIN11</t>
-  </si>
-  <si>
-    <t>BFRM11</t>
-  </si>
-  <si>
     <t>BMLC11</t>
   </si>
   <si>
-    <t>BPCA11</t>
-  </si>
-  <si>
     <t>BPFF11</t>
   </si>
   <si>
@@ -111,10 +72,241 @@
     <t>BRCR11</t>
   </si>
   <si>
-    <t>BRFI11</t>
-  </si>
-  <si>
     <t>CBOP11</t>
+  </si>
+  <si>
+    <t>CEOC11</t>
+  </si>
+  <si>
+    <t>CPTS11</t>
+  </si>
+  <si>
+    <t>CXRI11</t>
+  </si>
+  <si>
+    <t>DOMC11</t>
+  </si>
+  <si>
+    <t>EDGA11</t>
+  </si>
+  <si>
+    <t>FAED11</t>
+  </si>
+  <si>
+    <t>FIGS11</t>
+  </si>
+  <si>
+    <t>FISC11</t>
+  </si>
+  <si>
+    <t>FLMA11</t>
+  </si>
+  <si>
+    <t>FOFT11</t>
+  </si>
+  <si>
+    <t>FPAB11</t>
+  </si>
+  <si>
+    <t>FPNG11</t>
+  </si>
+  <si>
+    <t>FVPQ11</t>
+  </si>
+  <si>
+    <t>GGRC11</t>
+  </si>
+  <si>
+    <t>GRLV11</t>
+  </si>
+  <si>
+    <t>GTWR11</t>
+  </si>
+  <si>
+    <t>HABT11</t>
+  </si>
+  <si>
+    <t>HCRI11</t>
+  </si>
+  <si>
+    <t>HGCR11</t>
+  </si>
+  <si>
+    <t>HGLG11</t>
+  </si>
+  <si>
+    <t>HGRE11</t>
+  </si>
+  <si>
+    <t>HMOC11</t>
+  </si>
+  <si>
+    <t>HOSI11</t>
+  </si>
+  <si>
+    <t>HSML11</t>
+  </si>
+  <si>
+    <t>HTMX11</t>
+  </si>
+  <si>
+    <t>IBFF11</t>
+  </si>
+  <si>
+    <t>IRDM11</t>
+  </si>
+  <si>
+    <t>JPPC11</t>
+  </si>
+  <si>
+    <t>JRDM11</t>
+  </si>
+  <si>
+    <t>JSRE11</t>
+  </si>
+  <si>
+    <t>KNIP11</t>
+  </si>
+  <si>
+    <t>KNRE11</t>
+  </si>
+  <si>
+    <t>KNRI11</t>
+  </si>
+  <si>
+    <t>LASC11</t>
+  </si>
+  <si>
+    <t>LGCP11</t>
+  </si>
+  <si>
+    <t>LUGG11</t>
+  </si>
+  <si>
+    <t>LVBI11</t>
+  </si>
+  <si>
+    <t>MALL11</t>
+  </si>
+  <si>
+    <t>MAXR11</t>
+  </si>
+  <si>
+    <t>MFII11</t>
+  </si>
+  <si>
+    <t>MGFF11</t>
+  </si>
+  <si>
+    <t>MGHT11</t>
+  </si>
+  <si>
+    <t>MXRF11</t>
+  </si>
+  <si>
+    <t>NCHB11</t>
+  </si>
+  <si>
+    <t>NSLU11</t>
+  </si>
+  <si>
+    <t>NVHO11</t>
+  </si>
+  <si>
+    <t>ONEF11</t>
+  </si>
+  <si>
+    <t>OULG11</t>
+  </si>
+  <si>
+    <t>OUJP11</t>
+  </si>
+  <si>
+    <t>PATC11</t>
+  </si>
+  <si>
+    <t>PORD11</t>
+  </si>
+  <si>
+    <t>PRSV11</t>
+  </si>
+  <si>
+    <t>PVBI11</t>
+  </si>
+  <si>
+    <t>RBDS11</t>
+  </si>
+  <si>
+    <t>RBED11</t>
+  </si>
+  <si>
+    <t>RBFF11</t>
+  </si>
+  <si>
+    <t>RBGS11</t>
+  </si>
+  <si>
+    <t>RBRD11</t>
+  </si>
+  <si>
+    <t>RBVA11</t>
+  </si>
+  <si>
+    <t>RECT11</t>
+  </si>
+  <si>
+    <t>REIT11</t>
+  </si>
+  <si>
+    <t>RNGO11</t>
+  </si>
+  <si>
+    <t>SAAG11</t>
+  </si>
+  <si>
+    <t>SADI11</t>
+  </si>
+  <si>
+    <t>SARE11</t>
+  </si>
+  <si>
+    <t>SDIL11</t>
+  </si>
+  <si>
+    <t>SPTW11</t>
+  </si>
+  <si>
+    <t>TGAR11</t>
+  </si>
+  <si>
+    <t>TORD11</t>
+  </si>
+  <si>
+    <t>TRNT11</t>
+  </si>
+  <si>
+    <t>URPR11</t>
+  </si>
+  <si>
+    <t>VGIP11</t>
+  </si>
+  <si>
+    <t>VILG11</t>
+  </si>
+  <si>
+    <t>VISC11</t>
+  </si>
+  <si>
+    <t>VLOL11</t>
+  </si>
+  <si>
+    <t>VOTS11</t>
+  </si>
+  <si>
+    <t>VRTA11</t>
+  </si>
+  <si>
+    <t>WPLZ11</t>
   </si>
 </sst>
 </file>
@@ -175,6 +367,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -474,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD153"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -560,82 +756,467 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>